<commit_message>
updated WRCS appendix data and plots
</commit_message>
<xml_diff>
--- a/Salmonids/data/HatcheryWinterRunSurvival.xlsx
+++ b/Salmonids/data/HatcheryWinterRunSurvival.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/GitHub/omr_report_2024/Salmonids/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/GitHub/omr-report-2025/Salmonids/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{3F94AA43-D5D5-4318-BF8A-9534D8FB3D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60BFE22E-26F4-413A-8767-C9B60C27BF7C}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{3F94AA43-D5D5-4318-BF8A-9534D8FB3D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF5DAF0A-C636-40A3-A8F1-1B0F1BA87B09}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0F8A84CD-BEC0-46C5-BE5E-DA9E563ECAF4}"/>
+    <workbookView xWindow="945" yWindow="1155" windowWidth="21600" windowHeight="12270" xr2:uid="{0F8A84CD-BEC0-46C5-BE5E-DA9E563ECAF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>WY</t>
   </si>
@@ -154,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -164,6 +164,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6A8C4C-42FD-48B9-AC2F-1F2EEBB513AA}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +575,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:B12" si="0">C3-1</f>
+        <f t="shared" ref="B3:B13" si="0">C3-1</f>
         <v>2020</v>
       </c>
       <c r="C3" s="2">
@@ -668,30 +672,27 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" si="0"/>
-        <v>2018</v>
+        <v>2024</v>
       </c>
       <c r="C7" s="2">
-        <v>2019</v>
+        <v>2025</v>
       </c>
       <c r="D7" s="4">
-        <v>25.6</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="E7" s="5">
-        <v>1.7</v>
+        <v>2.8</v>
       </c>
       <c r="F7" s="5">
-        <v>22.4</v>
+        <v>58.5</v>
       </c>
       <c r="G7" s="5">
-        <v>29.1</v>
-      </c>
-      <c r="H7" s="5">
-        <v>90.2</v>
-      </c>
+        <v>69.3</v>
+      </c>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -699,25 +700,25 @@
       </c>
       <c r="B8" s="2">
         <f t="shared" si="0"/>
+        <v>2018</v>
+      </c>
+      <c r="C8" s="2">
         <v>2019</v>
       </c>
-      <c r="C8" s="2">
-        <v>2020</v>
-      </c>
       <c r="D8" s="4">
-        <v>3.5</v>
+        <v>25.6</v>
       </c>
       <c r="E8" s="5">
-        <v>0.9</v>
+        <v>1.7</v>
       </c>
       <c r="F8" s="5">
-        <v>2.2000000000000002</v>
+        <v>22.4</v>
       </c>
       <c r="G8" s="5">
-        <v>5.6</v>
+        <v>29.1</v>
       </c>
       <c r="H8" s="5">
-        <v>84.6</v>
+        <v>90.2</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -726,25 +727,25 @@
       </c>
       <c r="B9" s="2">
         <f t="shared" si="0"/>
+        <v>2019</v>
+      </c>
+      <c r="C9" s="2">
         <v>2020</v>
       </c>
-      <c r="C9" s="2">
-        <v>2021</v>
-      </c>
       <c r="D9" s="4">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="E9" s="5">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="F9" s="5">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G9" s="5">
-        <v>5.5</v>
+        <v>5.6</v>
       </c>
       <c r="H9" s="5">
-        <v>80</v>
+        <v>84.6</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -753,25 +754,25 @@
       </c>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="C10" s="2">
         <v>2021</v>
       </c>
-      <c r="C10" s="2">
-        <v>2022</v>
-      </c>
-      <c r="D10" s="6">
-        <v>5.8</v>
+      <c r="D10" s="4">
+        <v>3.6</v>
       </c>
       <c r="E10" s="5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F10" s="5">
-        <v>4.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G10" s="5">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="H10" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -780,25 +781,25 @@
       </c>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="C11" s="2">
         <v>2022</v>
       </c>
-      <c r="C11" s="2">
-        <v>2023</v>
-      </c>
-      <c r="D11" s="4">
-        <v>19.600000000000001</v>
+      <c r="D11" s="6">
+        <v>5.8</v>
       </c>
       <c r="E11" s="5">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="F11" s="5">
-        <v>17.100000000000001</v>
+        <v>4.2</v>
       </c>
       <c r="G11" s="5">
-        <v>22.4</v>
+        <v>8</v>
       </c>
       <c r="H11" s="5">
-        <v>97.3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -807,25 +808,78 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="C12" s="2">
         <v>2023</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="4">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="F12" s="5">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="G12" s="5">
+        <v>22.4</v>
+      </c>
+      <c r="H12" s="5">
+        <v>97.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="C13" s="2">
         <v>2024</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D13" s="4">
         <v>26.3</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E13" s="5">
         <v>1.8</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F13" s="5">
         <v>22.8</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G13" s="5">
         <v>30</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H13" s="5">
         <v>98.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7">
+        <v>2024</v>
+      </c>
+      <c r="C14" s="8">
+        <v>2025</v>
+      </c>
+      <c r="D14" s="9">
+        <v>26.7</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="10">
+        <v>23.8</v>
+      </c>
+      <c r="G14" s="10">
+        <v>29.7</v>
+      </c>
+      <c r="H14" s="10">
+        <v>93.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code updates to salmon and controlling factors
</commit_message>
<xml_diff>
--- a/Salmonids/data/HatcheryWinterRunSurvival.xlsx
+++ b/Salmonids/data/HatcheryWinterRunSurvival.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/GitHub/omr-report-2025/Salmonids/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cehlo_usbr_gov/Documents/LTO_2024_on/omr-report-2025/Salmonids/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{3F94AA43-D5D5-4318-BF8A-9534D8FB3D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF5DAF0A-C636-40A3-A8F1-1B0F1BA87B09}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="8_{3F94AA43-D5D5-4318-BF8A-9534D8FB3D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3621505E-972B-4375-86F0-552A435C5C3C}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="1155" windowWidth="21600" windowHeight="12270" xr2:uid="{0F8A84CD-BEC0-46C5-BE5E-DA9E563ECAF4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F8A84CD-BEC0-46C5-BE5E-DA9E563ECAF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>WY</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>BY</t>
+  </si>
+  <si>
+    <t>Entry</t>
   </si>
 </sst>
 </file>
@@ -114,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -150,11 +153,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -168,6 +200,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6A8C4C-42FD-48B9-AC2F-1F2EEBB513AA}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,6 +918,173 @@
         <v>93.8</v>
       </c>
     </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2">
+        <f>C15-1</f>
+        <v>2019</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D15" s="11">
+        <v>13.2</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="F15" s="12">
+        <v>10.5</v>
+      </c>
+      <c r="G15" s="12">
+        <v>16.5</v>
+      </c>
+      <c r="H15" s="12">
+        <v>93.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" ref="B16:B19" si="1">C16-1</f>
+        <v>2020</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2021</v>
+      </c>
+      <c r="D16">
+        <v>10.1</v>
+      </c>
+      <c r="E16">
+        <v>1.3</v>
+      </c>
+      <c r="F16" s="12">
+        <v>7.8</v>
+      </c>
+      <c r="G16" s="12">
+        <v>12.9</v>
+      </c>
+      <c r="H16" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" si="1"/>
+        <v>2021</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2022</v>
+      </c>
+      <c r="D17" s="13">
+        <v>13.4</v>
+      </c>
+      <c r="E17" s="14">
+        <v>1.4</v>
+      </c>
+      <c r="F17" s="12">
+        <v>10.8</v>
+      </c>
+      <c r="G17" s="12">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="H17" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="1"/>
+        <v>2022</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D18" s="13">
+        <v>14</v>
+      </c>
+      <c r="E18" s="14">
+        <v>1.3</v>
+      </c>
+      <c r="F18" s="12">
+        <v>11.7</v>
+      </c>
+      <c r="G18" s="12">
+        <v>16.8</v>
+      </c>
+      <c r="H18" s="12">
+        <v>64.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="1"/>
+        <v>2023</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2024</v>
+      </c>
+      <c r="D19" s="13">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="E19" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="F19" s="12">
+        <v>31.3</v>
+      </c>
+      <c r="G19" s="12">
+        <v>39.5</v>
+      </c>
+      <c r="H19" s="12">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D20">
+        <v>38</v>
+      </c>
+      <c r="E20">
+        <v>1.8</v>
+      </c>
+      <c r="F20">
+        <v>34.4</v>
+      </c>
+      <c r="G20">
+        <v>41.6</v>
+      </c>
+      <c r="H20">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <f>AVERAGE(D15:D20)</f>
+        <v>20.666666666666668</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>